<commit_message>
feat(database): Auto trim configuration parameter added
</commit_message>
<xml_diff>
--- a/plugins/db-wakamiti-plugin/src/test/resources/data2.xlsx
+++ b/plugins/db-wakamiti-plugin/src/test/resources/data2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgalbis\Proyectos\temp\plugins\db-wakamiti-plugin\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB11A656-C470-4735-8982-C53756187C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E3EE8A-199D-4345-9BE0-736026C74268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
     <t>2024-07-22 12:34:56</t>
   </si>
   <si>
-    <t>false</t>
+    <t>true</t>
   </si>
 </sst>
 </file>

</xml_diff>